<commit_message>
1.seller and client name wrap line in invoice and correction 2.set invoice and bill status PENDING only if current is DRAFT
</commit_message>
<xml_diff>
--- a/ArtTel/WebContent/data/reportTemplate/CorrectionTemplate.xlsx
+++ b/ArtTel/WebContent/data/reportTemplate/CorrectionTemplate.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="525" yWindow="3840" windowWidth="19470" windowHeight="6555"/>
+    <workbookView xWindow="525" yWindow="3840" windowWidth="19440" windowHeight="6555"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="2" r:id="rId1"/>
@@ -1021,75 +1021,52 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1099,64 +1076,45 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1189,75 +1147,105 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1277,16 +1265,16 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1295,30 +1283,12 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1336,6 +1306,42 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1636,8 +1642,8 @@
   </sheetPr>
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:B29"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1663,90 +1669,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="52.5" customHeight="1" thickBot="1">
-      <c r="A1" s="114"/>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="109" t="s">
+      <c r="A1" s="45"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="109"/>
-      <c r="G1" s="109"/>
-      <c r="H1" s="109"/>
-      <c r="I1" s="109"/>
-      <c r="J1" s="109"/>
-      <c r="K1" s="110"/>
-      <c r="L1" s="111"/>
-      <c r="M1" s="112"/>
-      <c r="N1" s="112"/>
-      <c r="O1" s="113"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="44"/>
     </row>
     <row r="2" spans="1:15" ht="18.75" customHeight="1">
-      <c r="A2" s="114"/>
-      <c r="B2" s="114"/>
-      <c r="C2" s="114"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="99" t="s">
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="77" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="100"/>
-      <c r="I2" s="100"/>
-      <c r="J2" s="100"/>
-      <c r="K2" s="101"/>
-      <c r="L2" s="132"/>
-      <c r="M2" s="133"/>
-      <c r="N2" s="133"/>
-      <c r="O2" s="134"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="79"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="64"/>
+      <c r="N2" s="64"/>
+      <c r="O2" s="65"/>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="114"/>
-      <c r="B3" s="114"/>
-      <c r="C3" s="114"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="135" t="s">
+      <c r="A3" s="45"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="136"/>
-      <c r="G3" s="136"/>
-      <c r="H3" s="136"/>
-      <c r="I3" s="136"/>
-      <c r="J3" s="136"/>
-      <c r="K3" s="137"/>
-      <c r="L3" s="93" t="s">
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="M3" s="94"/>
-      <c r="N3" s="94"/>
-      <c r="O3" s="95"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="72"/>
+      <c r="O3" s="73"/>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="116"/>
-      <c r="B4" s="116"/>
-      <c r="C4" s="116"/>
-      <c r="D4" s="117"/>
-      <c r="E4" s="138" t="s">
+      <c r="A4" s="47"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="138"/>
-      <c r="G4" s="138"/>
-      <c r="H4" s="138"/>
-      <c r="I4" s="138"/>
-      <c r="J4" s="138"/>
-      <c r="K4" s="139"/>
-      <c r="L4" s="96"/>
-      <c r="M4" s="97"/>
-      <c r="N4" s="97"/>
-      <c r="O4" s="98"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="69"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="69"/>
+      <c r="K4" s="70"/>
+      <c r="L4" s="74"/>
+      <c r="M4" s="75"/>
+      <c r="N4" s="75"/>
+      <c r="O4" s="76"/>
     </row>
     <row r="5" spans="1:15" ht="13.5" thickBot="1">
-      <c r="A5" s="118" t="s">
+      <c r="A5" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="119"/>
-      <c r="C5" s="119"/>
-      <c r="D5" s="119"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="L5" s="27"/>
@@ -1755,186 +1761,186 @@
       <c r="O5" s="28"/>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="120" t="s">
+      <c r="A6" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="121"/>
-      <c r="C6" s="121"/>
-      <c r="D6" s="121"/>
-      <c r="E6" s="122"/>
-      <c r="F6" s="120" t="s">
+      <c r="B6" s="55"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="121"/>
-      <c r="H6" s="121"/>
-      <c r="I6" s="102"/>
-      <c r="J6" s="102"/>
-      <c r="K6" s="102"/>
-      <c r="L6" s="102"/>
-      <c r="M6" s="102"/>
-      <c r="N6" s="102"/>
-      <c r="O6" s="103"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="80"/>
+      <c r="J6" s="80"/>
+      <c r="K6" s="80"/>
+      <c r="L6" s="80"/>
+      <c r="M6" s="80"/>
+      <c r="N6" s="80"/>
+      <c r="O6" s="81"/>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" s="123"/>
-      <c r="B7" s="124"/>
-      <c r="C7" s="124"/>
-      <c r="D7" s="124"/>
-      <c r="E7" s="125"/>
-      <c r="F7" s="123"/>
-      <c r="G7" s="124"/>
-      <c r="H7" s="124"/>
-      <c r="I7" s="124"/>
-      <c r="J7" s="124"/>
-      <c r="K7" s="124"/>
-      <c r="L7" s="124"/>
-      <c r="M7" s="124"/>
-      <c r="N7" s="124"/>
-      <c r="O7" s="125"/>
+      <c r="A7" s="164"/>
+      <c r="B7" s="165"/>
+      <c r="C7" s="165"/>
+      <c r="D7" s="165"/>
+      <c r="E7" s="166"/>
+      <c r="F7" s="164"/>
+      <c r="G7" s="165"/>
+      <c r="H7" s="165"/>
+      <c r="I7" s="165"/>
+      <c r="J7" s="165"/>
+      <c r="K7" s="165"/>
+      <c r="L7" s="165"/>
+      <c r="M7" s="165"/>
+      <c r="N7" s="165"/>
+      <c r="O7" s="166"/>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="123"/>
-      <c r="B8" s="124"/>
-      <c r="C8" s="124"/>
-      <c r="D8" s="124"/>
-      <c r="E8" s="125"/>
-      <c r="F8" s="123"/>
-      <c r="G8" s="124"/>
-      <c r="H8" s="124"/>
-      <c r="I8" s="124"/>
-      <c r="J8" s="124"/>
-      <c r="K8" s="124"/>
-      <c r="L8" s="124"/>
-      <c r="M8" s="124"/>
-      <c r="N8" s="124"/>
-      <c r="O8" s="125"/>
+      <c r="A8" s="164"/>
+      <c r="B8" s="165"/>
+      <c r="C8" s="165"/>
+      <c r="D8" s="165"/>
+      <c r="E8" s="166"/>
+      <c r="F8" s="164"/>
+      <c r="G8" s="165"/>
+      <c r="H8" s="165"/>
+      <c r="I8" s="165"/>
+      <c r="J8" s="165"/>
+      <c r="K8" s="165"/>
+      <c r="L8" s="165"/>
+      <c r="M8" s="165"/>
+      <c r="N8" s="165"/>
+      <c r="O8" s="166"/>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="123"/>
-      <c r="B9" s="124"/>
-      <c r="C9" s="124"/>
-      <c r="D9" s="124"/>
-      <c r="E9" s="125"/>
-      <c r="F9" s="123"/>
-      <c r="G9" s="124"/>
-      <c r="H9" s="124"/>
-      <c r="I9" s="124"/>
-      <c r="J9" s="124"/>
-      <c r="K9" s="124"/>
-      <c r="L9" s="124"/>
-      <c r="M9" s="124"/>
-      <c r="N9" s="124"/>
-      <c r="O9" s="125"/>
+      <c r="A9" s="164"/>
+      <c r="B9" s="165"/>
+      <c r="C9" s="165"/>
+      <c r="D9" s="165"/>
+      <c r="E9" s="166"/>
+      <c r="F9" s="164"/>
+      <c r="G9" s="165"/>
+      <c r="H9" s="165"/>
+      <c r="I9" s="165"/>
+      <c r="J9" s="165"/>
+      <c r="K9" s="165"/>
+      <c r="L9" s="165"/>
+      <c r="M9" s="165"/>
+      <c r="N9" s="165"/>
+      <c r="O9" s="166"/>
     </row>
     <row r="10" spans="1:15" ht="13.5" thickBot="1">
-      <c r="A10" s="126" t="s">
+      <c r="A10" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="127"/>
-      <c r="C10" s="127"/>
-      <c r="D10" s="127"/>
-      <c r="E10" s="128"/>
-      <c r="F10" s="126" t="s">
+      <c r="B10" s="58"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="127"/>
-      <c r="H10" s="127"/>
-      <c r="I10" s="127"/>
-      <c r="J10" s="127"/>
-      <c r="K10" s="127"/>
-      <c r="L10" s="127"/>
-      <c r="M10" s="127"/>
-      <c r="N10" s="127"/>
-      <c r="O10" s="128"/>
+      <c r="G10" s="58"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="58"/>
+      <c r="K10" s="58"/>
+      <c r="L10" s="58"/>
+      <c r="M10" s="58"/>
+      <c r="N10" s="58"/>
+      <c r="O10" s="59"/>
     </row>
     <row r="11" spans="1:15" ht="27.75" customHeight="1" thickBot="1">
-      <c r="A11" s="129" t="s">
+      <c r="A11" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="130"/>
-      <c r="C11" s="130"/>
-      <c r="D11" s="130"/>
-      <c r="E11" s="131"/>
-      <c r="F11" s="130" t="s">
+      <c r="B11" s="61"/>
+      <c r="C11" s="61"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="130"/>
-      <c r="H11" s="130"/>
-      <c r="I11" s="130"/>
-      <c r="J11" s="130"/>
-      <c r="K11" s="130"/>
-      <c r="L11" s="130"/>
-      <c r="M11" s="130"/>
-      <c r="N11" s="130"/>
-      <c r="O11" s="131"/>
+      <c r="G11" s="61"/>
+      <c r="H11" s="61"/>
+      <c r="I11" s="61"/>
+      <c r="J11" s="61"/>
+      <c r="K11" s="61"/>
+      <c r="L11" s="61"/>
+      <c r="M11" s="61"/>
+      <c r="N11" s="61"/>
+      <c r="O11" s="62"/>
     </row>
     <row r="12" spans="1:15" ht="6" customHeight="1" thickBot="1">
       <c r="A12" s="3"/>
       <c r="O12" s="4"/>
     </row>
     <row r="13" spans="1:15" s="5" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A13" s="104" t="s">
+      <c r="A13" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="60" t="s">
+      <c r="B13" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="60" t="s">
+      <c r="C13" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="60"/>
-      <c r="E13" s="60" t="s">
+      <c r="D13" s="51"/>
+      <c r="E13" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="107" t="s">
+      <c r="F13" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="82" t="s">
+      <c r="G13" s="105" t="s">
         <v>4</v>
       </c>
-      <c r="H13" s="82"/>
-      <c r="I13" s="76" t="s">
+      <c r="H13" s="105"/>
+      <c r="I13" s="99" t="s">
         <v>23</v>
       </c>
-      <c r="J13" s="80"/>
-      <c r="K13" s="82" t="s">
+      <c r="J13" s="103"/>
+      <c r="K13" s="105" t="s">
         <v>5</v>
       </c>
-      <c r="L13" s="82"/>
-      <c r="M13" s="82"/>
-      <c r="N13" s="76" t="s">
+      <c r="L13" s="105"/>
+      <c r="M13" s="105"/>
+      <c r="N13" s="99" t="s">
         <v>22</v>
       </c>
-      <c r="O13" s="77"/>
+      <c r="O13" s="100"/>
     </row>
     <row r="14" spans="1:15" s="6" customFormat="1">
-      <c r="A14" s="105"/>
-      <c r="B14" s="61"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="61"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="108"/>
-      <c r="G14" s="83"/>
-      <c r="H14" s="83"/>
-      <c r="I14" s="78"/>
-      <c r="J14" s="81"/>
+      <c r="A14" s="83"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="86"/>
+      <c r="G14" s="106"/>
+      <c r="H14" s="106"/>
+      <c r="I14" s="101"/>
+      <c r="J14" s="104"/>
       <c r="K14" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="L14" s="72" t="s">
+      <c r="L14" s="114" t="s">
         <v>7</v>
       </c>
-      <c r="M14" s="72"/>
-      <c r="N14" s="78"/>
-      <c r="O14" s="79"/>
+      <c r="M14" s="114"/>
+      <c r="N14" s="101"/>
+      <c r="O14" s="102"/>
     </row>
     <row r="15" spans="1:15" s="6" customFormat="1">
-      <c r="A15" s="106"/>
-      <c r="B15" s="62"/>
-      <c r="C15" s="62"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="108"/>
+      <c r="A15" s="84"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="86"/>
       <c r="G15" s="12" t="s">
         <v>8</v>
       </c>
@@ -1962,7 +1968,7 @@
       </c>
     </row>
     <row r="16" spans="1:15" s="6" customFormat="1">
-      <c r="A16" s="51"/>
+      <c r="A16" s="117"/>
       <c r="B16" s="21"/>
       <c r="C16" s="22"/>
       <c r="D16" s="26" t="s">
@@ -1970,53 +1976,53 @@
       </c>
       <c r="E16" s="22"/>
       <c r="F16" s="23"/>
-      <c r="G16" s="65"/>
-      <c r="H16" s="67"/>
-      <c r="I16" s="68"/>
-      <c r="J16" s="69"/>
+      <c r="G16" s="107"/>
+      <c r="H16" s="108"/>
+      <c r="I16" s="115"/>
+      <c r="J16" s="116"/>
       <c r="K16" s="24"/>
-      <c r="L16" s="65"/>
-      <c r="M16" s="67"/>
-      <c r="N16" s="65"/>
-      <c r="O16" s="66"/>
+      <c r="L16" s="107"/>
+      <c r="M16" s="108"/>
+      <c r="N16" s="107"/>
+      <c r="O16" s="109"/>
     </row>
     <row r="17" spans="1:15" s="6" customFormat="1">
-      <c r="A17" s="52"/>
-      <c r="B17" s="54"/>
+      <c r="A17" s="118"/>
+      <c r="B17" s="120"/>
       <c r="C17" s="22"/>
       <c r="D17" s="26" t="s">
         <v>31</v>
       </c>
       <c r="E17" s="22"/>
       <c r="F17" s="23"/>
-      <c r="G17" s="65"/>
-      <c r="H17" s="67"/>
-      <c r="I17" s="68"/>
-      <c r="J17" s="69"/>
+      <c r="G17" s="107"/>
+      <c r="H17" s="108"/>
+      <c r="I17" s="115"/>
+      <c r="J17" s="116"/>
       <c r="K17" s="24"/>
-      <c r="L17" s="65"/>
-      <c r="M17" s="67"/>
-      <c r="N17" s="65"/>
-      <c r="O17" s="66"/>
+      <c r="L17" s="107"/>
+      <c r="M17" s="108"/>
+      <c r="N17" s="107"/>
+      <c r="O17" s="109"/>
     </row>
     <row r="18" spans="1:15" s="6" customFormat="1">
-      <c r="A18" s="53"/>
-      <c r="B18" s="55"/>
+      <c r="A18" s="119"/>
+      <c r="B18" s="121"/>
       <c r="C18" s="22"/>
       <c r="D18" s="26" t="s">
         <v>32</v>
       </c>
       <c r="E18" s="22"/>
       <c r="F18" s="23"/>
-      <c r="G18" s="65"/>
-      <c r="H18" s="67"/>
-      <c r="I18" s="68"/>
-      <c r="J18" s="69"/>
+      <c r="G18" s="107"/>
+      <c r="H18" s="108"/>
+      <c r="I18" s="115"/>
+      <c r="J18" s="116"/>
       <c r="K18" s="24"/>
-      <c r="L18" s="65"/>
-      <c r="M18" s="67"/>
-      <c r="N18" s="65"/>
-      <c r="O18" s="66"/>
+      <c r="L18" s="107"/>
+      <c r="M18" s="108"/>
+      <c r="N18" s="107"/>
+      <c r="O18" s="109"/>
     </row>
     <row r="19" spans="1:15">
       <c r="A19" s="16"/>
@@ -2025,19 +2031,19 @@
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
-      <c r="G19" s="87" t="s">
+      <c r="G19" s="89" t="s">
         <v>12</v>
       </c>
-      <c r="H19" s="88"/>
-      <c r="I19" s="73"/>
-      <c r="J19" s="73"/>
+      <c r="H19" s="90"/>
+      <c r="I19" s="87"/>
+      <c r="J19" s="87"/>
       <c r="K19" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="L19" s="73"/>
-      <c r="M19" s="73"/>
-      <c r="N19" s="73"/>
-      <c r="O19" s="86"/>
+      <c r="L19" s="87"/>
+      <c r="M19" s="87"/>
+      <c r="N19" s="87"/>
+      <c r="O19" s="88"/>
     </row>
     <row r="20" spans="1:15">
       <c r="A20" s="16"/>
@@ -2046,19 +2052,19 @@
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
-      <c r="G20" s="84" t="s">
+      <c r="G20" s="112" t="s">
         <v>35</v>
       </c>
-      <c r="H20" s="85"/>
-      <c r="I20" s="73"/>
-      <c r="J20" s="73"/>
+      <c r="H20" s="113"/>
+      <c r="I20" s="87"/>
+      <c r="J20" s="87"/>
       <c r="K20" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="L20" s="73"/>
-      <c r="M20" s="73"/>
-      <c r="N20" s="73"/>
-      <c r="O20" s="86"/>
+      <c r="L20" s="87"/>
+      <c r="M20" s="87"/>
+      <c r="N20" s="87"/>
+      <c r="O20" s="88"/>
     </row>
     <row r="21" spans="1:15" ht="13.5" thickBot="1">
       <c r="A21" s="16"/>
@@ -2067,62 +2073,62 @@
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
       <c r="F21" s="32"/>
-      <c r="G21" s="74" t="s">
+      <c r="G21" s="110" t="s">
         <v>36</v>
       </c>
-      <c r="H21" s="75"/>
-      <c r="I21" s="63"/>
-      <c r="J21" s="63"/>
+      <c r="H21" s="111"/>
+      <c r="I21" s="124"/>
+      <c r="J21" s="124"/>
       <c r="K21" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="L21" s="63"/>
-      <c r="M21" s="63"/>
-      <c r="N21" s="63"/>
-      <c r="O21" s="64"/>
+      <c r="L21" s="124"/>
+      <c r="M21" s="124"/>
+      <c r="N21" s="124"/>
+      <c r="O21" s="125"/>
     </row>
     <row r="22" spans="1:15">
-      <c r="A22" s="140"/>
+      <c r="A22" s="33"/>
       <c r="B22" s="29"/>
       <c r="C22" s="29"/>
       <c r="D22" s="29"/>
       <c r="E22" s="29"/>
       <c r="F22" s="29"/>
-      <c r="G22" s="33" t="s">
+      <c r="G22" s="127" t="s">
         <v>13</v>
       </c>
-      <c r="H22" s="34"/>
-      <c r="I22" s="89"/>
-      <c r="J22" s="90"/>
+      <c r="H22" s="128"/>
+      <c r="I22" s="95"/>
+      <c r="J22" s="96"/>
       <c r="K22" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="L22" s="91"/>
-      <c r="M22" s="90"/>
-      <c r="N22" s="91"/>
-      <c r="O22" s="92"/>
+      <c r="L22" s="97"/>
+      <c r="M22" s="96"/>
+      <c r="N22" s="97"/>
+      <c r="O22" s="98"/>
     </row>
     <row r="23" spans="1:15">
-      <c r="A23" s="140"/>
+      <c r="A23" s="33"/>
       <c r="B23" s="29"/>
       <c r="C23" s="29"/>
       <c r="D23" s="29"/>
       <c r="E23" s="29"/>
       <c r="F23" s="29"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="70"/>
-      <c r="J23" s="71"/>
+      <c r="G23" s="127"/>
+      <c r="H23" s="128"/>
+      <c r="I23" s="91"/>
+      <c r="J23" s="92"/>
       <c r="K23" s="8">
         <v>23</v>
       </c>
-      <c r="L23" s="56"/>
-      <c r="M23" s="71"/>
-      <c r="N23" s="56"/>
-      <c r="O23" s="57"/>
+      <c r="L23" s="93"/>
+      <c r="M23" s="92"/>
+      <c r="N23" s="93"/>
+      <c r="O23" s="94"/>
     </row>
     <row r="24" spans="1:15" ht="13.5" thickBot="1">
-      <c r="A24" s="140" t="s">
+      <c r="A24" s="33" t="s">
         <v>17</v>
       </c>
       <c r="B24" s="29"/>
@@ -2130,63 +2136,63 @@
       <c r="D24" s="29"/>
       <c r="E24" s="29"/>
       <c r="F24" s="29"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="70"/>
-      <c r="J24" s="71"/>
+      <c r="G24" s="127"/>
+      <c r="H24" s="128"/>
+      <c r="I24" s="91"/>
+      <c r="J24" s="92"/>
       <c r="K24" s="8">
         <v>8</v>
       </c>
-      <c r="L24" s="56"/>
-      <c r="M24" s="71"/>
-      <c r="N24" s="56"/>
-      <c r="O24" s="57"/>
+      <c r="L24" s="93"/>
+      <c r="M24" s="92"/>
+      <c r="N24" s="93"/>
+      <c r="O24" s="94"/>
     </row>
     <row r="25" spans="1:15">
-      <c r="A25" s="141"/>
-      <c r="B25" s="142"/>
-      <c r="C25" s="142"/>
-      <c r="D25" s="142"/>
-      <c r="E25" s="142"/>
-      <c r="F25" s="143"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="34"/>
-      <c r="I25" s="70"/>
-      <c r="J25" s="71"/>
+      <c r="A25" s="135"/>
+      <c r="B25" s="136"/>
+      <c r="C25" s="136"/>
+      <c r="D25" s="136"/>
+      <c r="E25" s="136"/>
+      <c r="F25" s="137"/>
+      <c r="G25" s="127"/>
+      <c r="H25" s="128"/>
+      <c r="I25" s="91"/>
+      <c r="J25" s="92"/>
       <c r="K25" s="8">
         <v>5</v>
       </c>
-      <c r="L25" s="56"/>
-      <c r="M25" s="71"/>
-      <c r="N25" s="56"/>
-      <c r="O25" s="57"/>
+      <c r="L25" s="93"/>
+      <c r="M25" s="92"/>
+      <c r="N25" s="93"/>
+      <c r="O25" s="94"/>
     </row>
     <row r="26" spans="1:15" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A26" s="144"/>
-      <c r="B26" s="145"/>
-      <c r="C26" s="145"/>
-      <c r="D26" s="145"/>
-      <c r="E26" s="145"/>
-      <c r="F26" s="146"/>
-      <c r="G26" s="35"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="58"/>
-      <c r="J26" s="59"/>
+      <c r="A26" s="138"/>
+      <c r="B26" s="139"/>
+      <c r="C26" s="139"/>
+      <c r="D26" s="139"/>
+      <c r="E26" s="139"/>
+      <c r="F26" s="140"/>
+      <c r="G26" s="129"/>
+      <c r="H26" s="130"/>
+      <c r="I26" s="122"/>
+      <c r="J26" s="123"/>
       <c r="K26" s="17">
         <v>0</v>
       </c>
-      <c r="L26" s="37"/>
-      <c r="M26" s="59"/>
-      <c r="N26" s="37"/>
-      <c r="O26" s="38"/>
+      <c r="L26" s="126"/>
+      <c r="M26" s="123"/>
+      <c r="N26" s="126"/>
+      <c r="O26" s="131"/>
     </row>
     <row r="27" spans="1:15" ht="4.5" customHeight="1" thickBot="1">
-      <c r="A27" s="147"/>
-      <c r="B27" s="147"/>
-      <c r="C27" s="147"/>
-      <c r="D27" s="147"/>
-      <c r="E27" s="147"/>
-      <c r="F27" s="147"/>
+      <c r="A27" s="34"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
       <c r="I27" s="10"/>
       <c r="J27" s="10"/>
       <c r="K27" s="11"/>
@@ -2196,14 +2202,14 @@
       <c r="O27" s="10"/>
     </row>
     <row r="28" spans="1:15">
-      <c r="A28" s="148" t="s">
+      <c r="A28" s="141" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="149"/>
-      <c r="C28" s="150"/>
-      <c r="D28" s="151"/>
-      <c r="E28" s="151"/>
-      <c r="F28" s="152"/>
+      <c r="B28" s="142"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="145"/>
+      <c r="E28" s="145"/>
+      <c r="F28" s="146"/>
       <c r="G28" s="18"/>
       <c r="H28" s="18"/>
       <c r="I28" s="18"/>
@@ -2215,12 +2221,12 @@
       <c r="O28" s="18"/>
     </row>
     <row r="29" spans="1:15" ht="13.5" thickBot="1">
-      <c r="A29" s="153"/>
-      <c r="B29" s="154"/>
-      <c r="C29" s="155"/>
-      <c r="D29" s="156"/>
-      <c r="E29" s="156"/>
-      <c r="F29" s="157"/>
+      <c r="A29" s="143"/>
+      <c r="B29" s="144"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="147"/>
+      <c r="E29" s="147"/>
+      <c r="F29" s="148"/>
       <c r="G29" s="18"/>
       <c r="H29" s="18"/>
       <c r="I29" s="18"/>
@@ -2232,12 +2238,12 @@
       <c r="O29" s="18"/>
     </row>
     <row r="30" spans="1:15" ht="3.75" customHeight="1" thickBot="1">
-      <c r="A30" s="158"/>
-      <c r="B30" s="159"/>
-      <c r="C30" s="160"/>
-      <c r="D30" s="160"/>
-      <c r="E30" s="160"/>
-      <c r="F30" s="160"/>
+      <c r="A30" s="37"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
       <c r="G30" s="19"/>
       <c r="H30" s="19"/>
       <c r="I30" s="19"/>
@@ -2249,126 +2255,192 @@
       <c r="O30" s="19"/>
     </row>
     <row r="31" spans="1:15">
-      <c r="A31" s="161" t="s">
+      <c r="A31" s="149" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="162"/>
-      <c r="C31" s="162"/>
-      <c r="D31" s="162"/>
-      <c r="E31" s="162"/>
-      <c r="F31" s="162"/>
-      <c r="G31" s="162"/>
-      <c r="H31" s="162"/>
-      <c r="I31" s="162"/>
-      <c r="J31" s="162"/>
-      <c r="K31" s="162"/>
-      <c r="L31" s="162"/>
-      <c r="M31" s="162"/>
-      <c r="N31" s="162"/>
-      <c r="O31" s="163"/>
+      <c r="B31" s="150"/>
+      <c r="C31" s="150"/>
+      <c r="D31" s="150"/>
+      <c r="E31" s="150"/>
+      <c r="F31" s="150"/>
+      <c r="G31" s="150"/>
+      <c r="H31" s="150"/>
+      <c r="I31" s="150"/>
+      <c r="J31" s="150"/>
+      <c r="K31" s="150"/>
+      <c r="L31" s="150"/>
+      <c r="M31" s="150"/>
+      <c r="N31" s="150"/>
+      <c r="O31" s="151"/>
     </row>
     <row r="32" spans="1:15" ht="13.5" thickBot="1">
-      <c r="A32" s="164"/>
-      <c r="B32" s="165"/>
-      <c r="C32" s="165"/>
-      <c r="D32" s="165"/>
-      <c r="E32" s="165"/>
-      <c r="F32" s="165"/>
-      <c r="G32" s="165"/>
-      <c r="H32" s="165"/>
-      <c r="I32" s="165"/>
-      <c r="J32" s="165"/>
-      <c r="K32" s="165"/>
-      <c r="L32" s="165"/>
-      <c r="M32" s="165"/>
-      <c r="N32" s="165"/>
-      <c r="O32" s="166"/>
+      <c r="A32" s="152"/>
+      <c r="B32" s="153"/>
+      <c r="C32" s="153"/>
+      <c r="D32" s="153"/>
+      <c r="E32" s="153"/>
+      <c r="F32" s="153"/>
+      <c r="G32" s="153"/>
+      <c r="H32" s="153"/>
+      <c r="I32" s="153"/>
+      <c r="J32" s="153"/>
+      <c r="K32" s="153"/>
+      <c r="L32" s="153"/>
+      <c r="M32" s="153"/>
+      <c r="N32" s="153"/>
+      <c r="O32" s="154"/>
     </row>
     <row r="33" spans="2:14" ht="4.5" customHeight="1" thickBot="1">
       <c r="B33" s="14"/>
       <c r="C33" s="25"/>
-      <c r="D33" s="41"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="41"/>
-      <c r="H33" s="41"/>
-      <c r="I33" s="40"/>
-      <c r="J33" s="40"/>
-      <c r="K33" s="40"/>
-      <c r="L33" s="40"/>
-      <c r="M33" s="40"/>
-      <c r="N33" s="40"/>
+      <c r="D33" s="134"/>
+      <c r="E33" s="134"/>
+      <c r="F33" s="134"/>
+      <c r="G33" s="134"/>
+      <c r="H33" s="134"/>
+      <c r="I33" s="133"/>
+      <c r="J33" s="133"/>
+      <c r="K33" s="133"/>
+      <c r="L33" s="133"/>
+      <c r="M33" s="133"/>
+      <c r="N33" s="133"/>
     </row>
     <row r="34" spans="2:14">
-      <c r="B34" s="42"/>
-      <c r="C34" s="43"/>
-      <c r="D34" s="44"/>
-      <c r="H34" s="42"/>
-      <c r="I34" s="43"/>
-      <c r="J34" s="43"/>
-      <c r="K34" s="43"/>
-      <c r="L34" s="43"/>
-      <c r="M34" s="43"/>
-      <c r="N34" s="44"/>
+      <c r="B34" s="155"/>
+      <c r="C34" s="156"/>
+      <c r="D34" s="157"/>
+      <c r="H34" s="155"/>
+      <c r="I34" s="156"/>
+      <c r="J34" s="156"/>
+      <c r="K34" s="156"/>
+      <c r="L34" s="156"/>
+      <c r="M34" s="156"/>
+      <c r="N34" s="157"/>
     </row>
     <row r="35" spans="2:14">
-      <c r="B35" s="45"/>
-      <c r="C35" s="46"/>
-      <c r="D35" s="47"/>
-      <c r="H35" s="45"/>
-      <c r="I35" s="46"/>
-      <c r="J35" s="46"/>
-      <c r="K35" s="46"/>
-      <c r="L35" s="46"/>
-      <c r="M35" s="46"/>
-      <c r="N35" s="47"/>
+      <c r="B35" s="158"/>
+      <c r="C35" s="159"/>
+      <c r="D35" s="160"/>
+      <c r="H35" s="158"/>
+      <c r="I35" s="159"/>
+      <c r="J35" s="159"/>
+      <c r="K35" s="159"/>
+      <c r="L35" s="159"/>
+      <c r="M35" s="159"/>
+      <c r="N35" s="160"/>
     </row>
     <row r="36" spans="2:14">
-      <c r="B36" s="45"/>
-      <c r="C36" s="46"/>
-      <c r="D36" s="47"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="46"/>
-      <c r="J36" s="46"/>
-      <c r="K36" s="46"/>
-      <c r="L36" s="46"/>
-      <c r="M36" s="46"/>
-      <c r="N36" s="47"/>
+      <c r="B36" s="158"/>
+      <c r="C36" s="159"/>
+      <c r="D36" s="160"/>
+      <c r="H36" s="158"/>
+      <c r="I36" s="159"/>
+      <c r="J36" s="159"/>
+      <c r="K36" s="159"/>
+      <c r="L36" s="159"/>
+      <c r="M36" s="159"/>
+      <c r="N36" s="160"/>
     </row>
     <row r="37" spans="2:14" ht="13.5" thickBot="1">
-      <c r="B37" s="48"/>
-      <c r="C37" s="49"/>
-      <c r="D37" s="50"/>
-      <c r="H37" s="48"/>
-      <c r="I37" s="49"/>
-      <c r="J37" s="49"/>
-      <c r="K37" s="49"/>
-      <c r="L37" s="49"/>
-      <c r="M37" s="49"/>
-      <c r="N37" s="50"/>
+      <c r="B37" s="161"/>
+      <c r="C37" s="162"/>
+      <c r="D37" s="163"/>
+      <c r="H37" s="161"/>
+      <c r="I37" s="162"/>
+      <c r="J37" s="162"/>
+      <c r="K37" s="162"/>
+      <c r="L37" s="162"/>
+      <c r="M37" s="162"/>
+      <c r="N37" s="163"/>
     </row>
     <row r="38" spans="2:14">
-      <c r="B38" s="39" t="s">
+      <c r="B38" s="132" t="s">
         <v>14</v>
       </c>
-      <c r="C38" s="39"/>
-      <c r="D38" s="39"/>
+      <c r="C38" s="132"/>
+      <c r="D38" s="132"/>
       <c r="E38" s="15"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15"/>
-      <c r="H38" s="39" t="s">
+      <c r="H38" s="132" t="s">
         <v>15</v>
       </c>
-      <c r="I38" s="39"/>
-      <c r="J38" s="39"/>
-      <c r="K38" s="39"/>
-      <c r="L38" s="39"/>
-      <c r="M38" s="39"/>
-      <c r="N38" s="39"/>
+      <c r="I38" s="132"/>
+      <c r="J38" s="132"/>
+      <c r="K38" s="132"/>
+      <c r="L38" s="132"/>
+      <c r="M38" s="132"/>
+      <c r="N38" s="132"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="82">
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="H38:N38"/>
+    <mergeCell ref="I33:N33"/>
+    <mergeCell ref="D33:H33"/>
+    <mergeCell ref="A25:F26"/>
+    <mergeCell ref="A28:B29"/>
+    <mergeCell ref="D28:F29"/>
+    <mergeCell ref="A31:O32"/>
+    <mergeCell ref="B34:D37"/>
+    <mergeCell ref="H34:N37"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H26"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="L3:O3"/>
+    <mergeCell ref="L4:O4"/>
+    <mergeCell ref="E2:K2"/>
+    <mergeCell ref="I6:O6"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="F13:F15"/>
+    <mergeCell ref="N13:O14"/>
+    <mergeCell ref="I13:J14"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="G13:H14"/>
+    <mergeCell ref="L14:M14"/>
     <mergeCell ref="E1:K1"/>
     <mergeCell ref="L1:O1"/>
     <mergeCell ref="A1:D4"/>
@@ -2385,72 +2457,6 @@
     <mergeCell ref="L2:O2"/>
     <mergeCell ref="E3:K3"/>
     <mergeCell ref="E4:K4"/>
-    <mergeCell ref="L3:O3"/>
-    <mergeCell ref="L4:O4"/>
-    <mergeCell ref="E2:K2"/>
-    <mergeCell ref="I6:O6"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="F13:F15"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="N13:O14"/>
-    <mergeCell ref="I13:J14"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="G13:H14"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="E13:E15"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="G22:H26"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="H38:N38"/>
-    <mergeCell ref="I33:N33"/>
-    <mergeCell ref="D33:H33"/>
-    <mergeCell ref="A25:F26"/>
-    <mergeCell ref="A28:B29"/>
-    <mergeCell ref="D28:F29"/>
-    <mergeCell ref="A31:O32"/>
-    <mergeCell ref="B34:D37"/>
-    <mergeCell ref="H34:N37"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="L25:M25"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
1. Minor changes in new PDF print invoice/correction generator based on FTL 2. Regulation drived changes in Invoice/Corrections: new unit types, new vat rates, document format changes 3. new PKWiU field in Product entity, included on invoice/correction document, Product DAO/Service refactoring
</commit_message>
<xml_diff>
--- a/ArtTel/WebContent/data/reportTemplate/CorrectionTemplate.xlsx
+++ b/ArtTel/WebContent/data/reportTemplate/CorrectionTemplate.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Arkusz1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>pieczęć sprzedawcy</t>
   </si>
@@ -93,13 +93,7 @@
     <t>x</t>
   </si>
   <si>
-    <t>zw</t>
-  </si>
-  <si>
     <t>RAZEM</t>
-  </si>
-  <si>
-    <t>W TYM</t>
   </si>
   <si>
     <t>podpis imienny osoby upoważnionej do odbioru faktur VAT</t>
@@ -951,7 +945,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="167">
+  <cellXfs count="173">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -966,7 +960,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -987,12 +980,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1014,12 +1005,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1042,31 +1027,156 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1076,45 +1186,49 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1147,18 +1261,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1183,165 +1285,81 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1640,17 +1658,17 @@
   <sheetPr codeName="Arkusz1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O38"/>
+  <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:F26"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="3.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="5.7109375" style="1" customWidth="1"/>
@@ -1658,7 +1676,7 @@
     <col min="8" max="8" width="5" style="1" customWidth="1"/>
     <col min="9" max="9" width="7.28515625" style="1" customWidth="1"/>
     <col min="10" max="10" width="4" style="1" customWidth="1"/>
-    <col min="11" max="11" width="3.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" style="1" customWidth="1"/>
     <col min="12" max="12" width="6.85546875" style="1" customWidth="1"/>
     <col min="13" max="13" width="2.42578125" style="1" customWidth="1"/>
     <col min="14" max="14" width="8.7109375" style="1" customWidth="1"/>
@@ -1669,740 +1687,718 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="52.5" customHeight="1" thickBot="1">
-      <c r="A1" s="45"/>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="44"/>
+      <c r="A1" s="147"/>
+      <c r="B1" s="147"/>
+      <c r="C1" s="147"/>
+      <c r="D1" s="148"/>
+      <c r="E1" s="142" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="142"/>
+      <c r="G1" s="142"/>
+      <c r="H1" s="142"/>
+      <c r="I1" s="142"/>
+      <c r="J1" s="142"/>
+      <c r="K1" s="143"/>
+      <c r="L1" s="144"/>
+      <c r="M1" s="145"/>
+      <c r="N1" s="145"/>
+      <c r="O1" s="146"/>
     </row>
     <row r="2" spans="1:15" ht="18.75" customHeight="1">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="77" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="63"/>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="O2" s="65"/>
+      <c r="A2" s="147"/>
+      <c r="B2" s="147"/>
+      <c r="C2" s="147"/>
+      <c r="D2" s="148"/>
+      <c r="E2" s="123" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="124"/>
+      <c r="G2" s="124"/>
+      <c r="H2" s="124"/>
+      <c r="I2" s="124"/>
+      <c r="J2" s="124"/>
+      <c r="K2" s="125"/>
+      <c r="L2" s="165"/>
+      <c r="M2" s="166"/>
+      <c r="N2" s="166"/>
+      <c r="O2" s="167"/>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="45"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="66" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="68"/>
-      <c r="L3" s="71" t="s">
+      <c r="A3" s="147"/>
+      <c r="B3" s="147"/>
+      <c r="C3" s="147"/>
+      <c r="D3" s="148"/>
+      <c r="E3" s="168" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="169"/>
+      <c r="G3" s="169"/>
+      <c r="H3" s="169"/>
+      <c r="I3" s="169"/>
+      <c r="J3" s="169"/>
+      <c r="K3" s="170"/>
+      <c r="L3" s="117" t="s">
         <v>1</v>
       </c>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
-      <c r="O3" s="73"/>
+      <c r="M3" s="118"/>
+      <c r="N3" s="118"/>
+      <c r="O3" s="119"/>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="47"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="69" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="69"/>
-      <c r="K4" s="70"/>
-      <c r="L4" s="74"/>
-      <c r="M4" s="75"/>
-      <c r="N4" s="75"/>
-      <c r="O4" s="76"/>
+      <c r="A4" s="149"/>
+      <c r="B4" s="149"/>
+      <c r="C4" s="149"/>
+      <c r="D4" s="150"/>
+      <c r="E4" s="171" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="171"/>
+      <c r="G4" s="171"/>
+      <c r="H4" s="171"/>
+      <c r="I4" s="171"/>
+      <c r="J4" s="171"/>
+      <c r="K4" s="172"/>
+      <c r="L4" s="120"/>
+      <c r="M4" s="121"/>
+      <c r="N4" s="121"/>
+      <c r="O4" s="122"/>
     </row>
     <row r="5" spans="1:15" ht="13.5" thickBot="1">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="151" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
+      <c r="B5" s="152"/>
+      <c r="C5" s="152"/>
+      <c r="D5" s="152"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="L5" s="27"/>
-      <c r="M5" s="27"/>
-      <c r="N5" s="27"/>
-      <c r="O5" s="28"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="25"/>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="54" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="54" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="80"/>
-      <c r="J6" s="80"/>
-      <c r="K6" s="80"/>
-      <c r="L6" s="80"/>
-      <c r="M6" s="80"/>
-      <c r="N6" s="80"/>
-      <c r="O6" s="81"/>
+      <c r="A6" s="153" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="154"/>
+      <c r="C6" s="154"/>
+      <c r="D6" s="154"/>
+      <c r="E6" s="155"/>
+      <c r="F6" s="153" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="154"/>
+      <c r="H6" s="154"/>
+      <c r="I6" s="126"/>
+      <c r="J6" s="126"/>
+      <c r="K6" s="126"/>
+      <c r="L6" s="126"/>
+      <c r="M6" s="126"/>
+      <c r="N6" s="126"/>
+      <c r="O6" s="127"/>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" s="164"/>
-      <c r="B7" s="165"/>
-      <c r="C7" s="165"/>
-      <c r="D7" s="165"/>
-      <c r="E7" s="166"/>
-      <c r="F7" s="164"/>
-      <c r="G7" s="165"/>
-      <c r="H7" s="165"/>
-      <c r="I7" s="165"/>
-      <c r="J7" s="165"/>
-      <c r="K7" s="165"/>
-      <c r="L7" s="165"/>
-      <c r="M7" s="165"/>
-      <c r="N7" s="165"/>
-      <c r="O7" s="166"/>
+      <c r="A7" s="156"/>
+      <c r="B7" s="157"/>
+      <c r="C7" s="157"/>
+      <c r="D7" s="157"/>
+      <c r="E7" s="158"/>
+      <c r="F7" s="156"/>
+      <c r="G7" s="157"/>
+      <c r="H7" s="157"/>
+      <c r="I7" s="157"/>
+      <c r="J7" s="157"/>
+      <c r="K7" s="157"/>
+      <c r="L7" s="157"/>
+      <c r="M7" s="157"/>
+      <c r="N7" s="157"/>
+      <c r="O7" s="158"/>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="164"/>
-      <c r="B8" s="165"/>
-      <c r="C8" s="165"/>
-      <c r="D8" s="165"/>
-      <c r="E8" s="166"/>
-      <c r="F8" s="164"/>
-      <c r="G8" s="165"/>
-      <c r="H8" s="165"/>
-      <c r="I8" s="165"/>
-      <c r="J8" s="165"/>
-      <c r="K8" s="165"/>
-      <c r="L8" s="165"/>
-      <c r="M8" s="165"/>
-      <c r="N8" s="165"/>
-      <c r="O8" s="166"/>
-    </row>
-    <row r="9" spans="1:15">
-      <c r="A9" s="164"/>
-      <c r="B9" s="165"/>
-      <c r="C9" s="165"/>
-      <c r="D9" s="165"/>
-      <c r="E9" s="166"/>
-      <c r="F9" s="164"/>
-      <c r="G9" s="165"/>
-      <c r="H9" s="165"/>
-      <c r="I9" s="165"/>
-      <c r="J9" s="165"/>
-      <c r="K9" s="165"/>
-      <c r="L9" s="165"/>
-      <c r="M9" s="165"/>
-      <c r="N9" s="165"/>
-      <c r="O9" s="166"/>
+      <c r="A8" s="156"/>
+      <c r="B8" s="157"/>
+      <c r="C8" s="157"/>
+      <c r="D8" s="157"/>
+      <c r="E8" s="158"/>
+      <c r="F8" s="156"/>
+      <c r="G8" s="157"/>
+      <c r="H8" s="157"/>
+      <c r="I8" s="157"/>
+      <c r="J8" s="157"/>
+      <c r="K8" s="157"/>
+      <c r="L8" s="157"/>
+      <c r="M8" s="157"/>
+      <c r="N8" s="157"/>
+      <c r="O8" s="158"/>
+    </row>
+    <row r="9" spans="1:15" ht="26.25" customHeight="1">
+      <c r="A9" s="156"/>
+      <c r="B9" s="157"/>
+      <c r="C9" s="157"/>
+      <c r="D9" s="157"/>
+      <c r="E9" s="158"/>
+      <c r="F9" s="156"/>
+      <c r="G9" s="157"/>
+      <c r="H9" s="157"/>
+      <c r="I9" s="157"/>
+      <c r="J9" s="157"/>
+      <c r="K9" s="157"/>
+      <c r="L9" s="157"/>
+      <c r="M9" s="157"/>
+      <c r="N9" s="157"/>
+      <c r="O9" s="158"/>
     </row>
     <row r="10" spans="1:15" ht="13.5" thickBot="1">
-      <c r="A10" s="57" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="58"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="57" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="58"/>
-      <c r="H10" s="58"/>
-      <c r="I10" s="58"/>
-      <c r="J10" s="58"/>
-      <c r="K10" s="58"/>
-      <c r="L10" s="58"/>
-      <c r="M10" s="58"/>
-      <c r="N10" s="58"/>
-      <c r="O10" s="59"/>
+      <c r="A10" s="159" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="160"/>
+      <c r="C10" s="160"/>
+      <c r="D10" s="160"/>
+      <c r="E10" s="161"/>
+      <c r="F10" s="159" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="160"/>
+      <c r="H10" s="160"/>
+      <c r="I10" s="160"/>
+      <c r="J10" s="160"/>
+      <c r="K10" s="160"/>
+      <c r="L10" s="160"/>
+      <c r="M10" s="160"/>
+      <c r="N10" s="160"/>
+      <c r="O10" s="161"/>
     </row>
     <row r="11" spans="1:15" ht="27.75" customHeight="1" thickBot="1">
-      <c r="A11" s="60" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="61"/>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11" s="61"/>
-      <c r="H11" s="61"/>
-      <c r="I11" s="61"/>
-      <c r="J11" s="61"/>
-      <c r="K11" s="61"/>
-      <c r="L11" s="61"/>
-      <c r="M11" s="61"/>
-      <c r="N11" s="61"/>
-      <c r="O11" s="62"/>
+      <c r="A11" s="162" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="163"/>
+      <c r="C11" s="163"/>
+      <c r="D11" s="163"/>
+      <c r="E11" s="164"/>
+      <c r="F11" s="163" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="163"/>
+      <c r="H11" s="163"/>
+      <c r="I11" s="163"/>
+      <c r="J11" s="163"/>
+      <c r="K11" s="163"/>
+      <c r="L11" s="163"/>
+      <c r="M11" s="163"/>
+      <c r="N11" s="163"/>
+      <c r="O11" s="164"/>
     </row>
     <row r="12" spans="1:15" ht="6" customHeight="1" thickBot="1">
       <c r="A12" s="3"/>
       <c r="O12" s="4"/>
     </row>
     <row r="13" spans="1:15" s="5" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A13" s="82" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="51" t="s">
+      <c r="A13" s="128" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="51" t="s">
+      <c r="C13" s="89" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="89"/>
+      <c r="E13" s="89" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="131" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="139" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" s="139"/>
+      <c r="I13" s="133" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51" t="s">
-        <v>3</v>
-      </c>
-      <c r="F13" s="85" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" s="105" t="s">
-        <v>4</v>
-      </c>
-      <c r="H13" s="105"/>
-      <c r="I13" s="99" t="s">
-        <v>23</v>
-      </c>
-      <c r="J13" s="103"/>
-      <c r="K13" s="105" t="s">
+      <c r="J13" s="137"/>
+      <c r="K13" s="139" t="s">
         <v>5</v>
       </c>
-      <c r="L13" s="105"/>
-      <c r="M13" s="105"/>
-      <c r="N13" s="99" t="s">
-        <v>22</v>
-      </c>
-      <c r="O13" s="100"/>
+      <c r="L13" s="139"/>
+      <c r="M13" s="139"/>
+      <c r="N13" s="133" t="s">
+        <v>20</v>
+      </c>
+      <c r="O13" s="134"/>
     </row>
     <row r="14" spans="1:15" s="6" customFormat="1">
-      <c r="A14" s="83"/>
-      <c r="B14" s="52"/>
-      <c r="C14" s="52"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="86"/>
-      <c r="G14" s="106"/>
-      <c r="H14" s="106"/>
-      <c r="I14" s="101"/>
-      <c r="J14" s="104"/>
-      <c r="K14" s="9" t="s">
+      <c r="A14" s="129"/>
+      <c r="B14" s="90"/>
+      <c r="C14" s="90"/>
+      <c r="D14" s="90"/>
+      <c r="E14" s="90"/>
+      <c r="F14" s="132"/>
+      <c r="G14" s="140"/>
+      <c r="H14" s="140"/>
+      <c r="I14" s="135"/>
+      <c r="J14" s="138"/>
+      <c r="K14" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="L14" s="114" t="s">
+      <c r="L14" s="141" t="s">
         <v>7</v>
       </c>
-      <c r="M14" s="114"/>
-      <c r="N14" s="101"/>
-      <c r="O14" s="102"/>
+      <c r="M14" s="141"/>
+      <c r="N14" s="135"/>
+      <c r="O14" s="136"/>
     </row>
     <row r="15" spans="1:15" s="6" customFormat="1">
-      <c r="A15" s="84"/>
-      <c r="B15" s="53"/>
-      <c r="C15" s="53"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="53"/>
-      <c r="F15" s="86"/>
-      <c r="G15" s="12" t="s">
+      <c r="A15" s="130"/>
+      <c r="B15" s="91"/>
+      <c r="C15" s="91"/>
+      <c r="D15" s="91"/>
+      <c r="E15" s="91"/>
+      <c r="F15" s="132"/>
+      <c r="G15" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="12" t="s">
+      <c r="H15" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I15" s="12" t="s">
+      <c r="I15" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J15" s="12" t="s">
+      <c r="J15" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12" t="s">
+      <c r="K15" s="11"/>
+      <c r="L15" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M15" s="12" t="s">
+      <c r="M15" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="N15" s="12" t="s">
+      <c r="N15" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="O15" s="13" t="s">
+      <c r="O15" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:15" s="6" customFormat="1">
-      <c r="A16" s="117"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="26" t="s">
+      <c r="A16" s="81"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="19"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="94"/>
+      <c r="H16" s="96"/>
+      <c r="I16" s="98"/>
+      <c r="J16" s="99"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="94"/>
+      <c r="M16" s="96"/>
+      <c r="N16" s="94"/>
+      <c r="O16" s="95"/>
+    </row>
+    <row r="17" spans="1:15" s="6" customFormat="1">
+      <c r="A17" s="82"/>
+      <c r="B17" s="84"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="19"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="94"/>
+      <c r="H17" s="96"/>
+      <c r="I17" s="98"/>
+      <c r="J17" s="99"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="94"/>
+      <c r="M17" s="96"/>
+      <c r="N17" s="94"/>
+      <c r="O17" s="95"/>
+    </row>
+    <row r="18" spans="1:15" s="6" customFormat="1">
+      <c r="A18" s="83"/>
+      <c r="B18" s="85"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="22"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="107"/>
-      <c r="H16" s="108"/>
-      <c r="I16" s="115"/>
-      <c r="J16" s="116"/>
-      <c r="K16" s="24"/>
-      <c r="L16" s="107"/>
-      <c r="M16" s="108"/>
-      <c r="N16" s="107"/>
-      <c r="O16" s="109"/>
-    </row>
-    <row r="17" spans="1:15" s="6" customFormat="1">
-      <c r="A17" s="118"/>
-      <c r="B17" s="120"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="22"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="107"/>
-      <c r="H17" s="108"/>
-      <c r="I17" s="115"/>
-      <c r="J17" s="116"/>
-      <c r="K17" s="24"/>
-      <c r="L17" s="107"/>
-      <c r="M17" s="108"/>
-      <c r="N17" s="107"/>
-      <c r="O17" s="109"/>
-    </row>
-    <row r="18" spans="1:15" s="6" customFormat="1">
-      <c r="A18" s="119"/>
-      <c r="B18" s="121"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" s="22"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="107"/>
-      <c r="H18" s="108"/>
-      <c r="I18" s="115"/>
-      <c r="J18" s="116"/>
-      <c r="K18" s="24"/>
-      <c r="L18" s="107"/>
-      <c r="M18" s="108"/>
-      <c r="N18" s="107"/>
-      <c r="O18" s="109"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="94"/>
+      <c r="H18" s="96"/>
+      <c r="I18" s="98"/>
+      <c r="J18" s="99"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="94"/>
+      <c r="M18" s="96"/>
+      <c r="N18" s="94"/>
+      <c r="O18" s="95"/>
     </row>
     <row r="19" spans="1:15">
-      <c r="A19" s="16"/>
+      <c r="A19" s="15"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
-      <c r="G19" s="89" t="s">
-        <v>12</v>
-      </c>
-      <c r="H19" s="90"/>
-      <c r="I19" s="87"/>
-      <c r="J19" s="87"/>
-      <c r="K19" s="30" t="s">
+      <c r="G19" s="104" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="105"/>
+      <c r="I19" s="100"/>
+      <c r="J19" s="100"/>
+      <c r="K19" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="L19" s="87"/>
-      <c r="M19" s="87"/>
-      <c r="N19" s="87"/>
-      <c r="O19" s="88"/>
+      <c r="L19" s="100"/>
+      <c r="M19" s="100"/>
+      <c r="N19" s="100"/>
+      <c r="O19" s="103"/>
     </row>
     <row r="20" spans="1:15">
-      <c r="A20" s="16"/>
+      <c r="A20" s="15"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
-      <c r="G20" s="112" t="s">
-        <v>35</v>
-      </c>
-      <c r="H20" s="113"/>
-      <c r="I20" s="87"/>
-      <c r="J20" s="87"/>
-      <c r="K20" s="30" t="s">
+      <c r="G20" s="101" t="s">
+        <v>33</v>
+      </c>
+      <c r="H20" s="102"/>
+      <c r="I20" s="100"/>
+      <c r="J20" s="100"/>
+      <c r="K20" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="L20" s="87"/>
-      <c r="M20" s="87"/>
-      <c r="N20" s="87"/>
-      <c r="O20" s="88"/>
+      <c r="L20" s="100"/>
+      <c r="M20" s="100"/>
+      <c r="N20" s="100"/>
+      <c r="O20" s="103"/>
     </row>
     <row r="21" spans="1:15" ht="13.5" thickBot="1">
-      <c r="A21" s="16"/>
+      <c r="A21" s="15"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="110" t="s">
-        <v>36</v>
-      </c>
-      <c r="H21" s="111"/>
-      <c r="I21" s="124"/>
-      <c r="J21" s="124"/>
-      <c r="K21" s="31" t="s">
+      <c r="F21" s="27"/>
+      <c r="G21" s="106" t="s">
+        <v>34</v>
+      </c>
+      <c r="H21" s="107"/>
+      <c r="I21" s="92"/>
+      <c r="J21" s="92"/>
+      <c r="K21" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="L21" s="124"/>
-      <c r="M21" s="124"/>
-      <c r="N21" s="124"/>
-      <c r="O21" s="125"/>
+      <c r="L21" s="92"/>
+      <c r="M21" s="92"/>
+      <c r="N21" s="92"/>
+      <c r="O21" s="93"/>
     </row>
     <row r="22" spans="1:15">
-      <c r="A22" s="33"/>
-      <c r="B22" s="29"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="127" t="s">
+      <c r="A22" s="28"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="108"/>
+      <c r="H22" s="109"/>
+      <c r="I22" s="113"/>
+      <c r="J22" s="114"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="115"/>
+      <c r="M22" s="114"/>
+      <c r="N22" s="115"/>
+      <c r="O22" s="116"/>
+    </row>
+    <row r="23" spans="1:15" ht="13.5" thickBot="1">
+      <c r="A23" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="108"/>
+      <c r="H23" s="109"/>
+      <c r="I23" s="72"/>
+      <c r="J23" s="73"/>
+      <c r="K23" s="38"/>
+      <c r="L23" s="74"/>
+      <c r="M23" s="73"/>
+      <c r="N23" s="74"/>
+      <c r="O23" s="86"/>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" s="43"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="108"/>
+      <c r="H24" s="109"/>
+      <c r="I24" s="72"/>
+      <c r="J24" s="73"/>
+      <c r="K24" s="38"/>
+      <c r="L24" s="74"/>
+      <c r="M24" s="73"/>
+      <c r="N24" s="74"/>
+      <c r="O24" s="86"/>
+    </row>
+    <row r="25" spans="1:15" ht="16.5" customHeight="1" thickBot="1">
+      <c r="A25" s="46"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="110"/>
+      <c r="H25" s="111"/>
+      <c r="I25" s="87"/>
+      <c r="J25" s="88"/>
+      <c r="K25" s="39"/>
+      <c r="L25" s="97"/>
+      <c r="M25" s="88"/>
+      <c r="N25" s="97"/>
+      <c r="O25" s="112"/>
+    </row>
+    <row r="26" spans="1:15" ht="4.5" customHeight="1" thickBot="1">
+      <c r="A26" s="29"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" s="50"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="53"/>
+      <c r="E27" s="53"/>
+      <c r="F27" s="54"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="75"/>
+      <c r="I27" s="76"/>
+      <c r="J27" s="76"/>
+      <c r="K27" s="76"/>
+      <c r="L27" s="76"/>
+      <c r="M27" s="76"/>
+      <c r="N27" s="76"/>
+      <c r="O27" s="77"/>
+    </row>
+    <row r="28" spans="1:15" ht="13.5" thickBot="1">
+      <c r="A28" s="51"/>
+      <c r="B28" s="52"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="55"/>
+      <c r="F28" s="56"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="78"/>
+      <c r="I28" s="79"/>
+      <c r="J28" s="79"/>
+      <c r="K28" s="79"/>
+      <c r="L28" s="79"/>
+      <c r="M28" s="79"/>
+      <c r="N28" s="79"/>
+      <c r="O28" s="80"/>
+    </row>
+    <row r="29" spans="1:15" ht="3.75" customHeight="1" thickBot="1">
+      <c r="A29" s="32"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="17"/>
+      <c r="O29" s="17"/>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="A30" s="57" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="58"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="58"/>
+      <c r="E30" s="58"/>
+      <c r="F30" s="58"/>
+      <c r="G30" s="58"/>
+      <c r="H30" s="58"/>
+      <c r="I30" s="58"/>
+      <c r="J30" s="58"/>
+      <c r="K30" s="58"/>
+      <c r="L30" s="58"/>
+      <c r="M30" s="58"/>
+      <c r="N30" s="58"/>
+      <c r="O30" s="59"/>
+    </row>
+    <row r="31" spans="1:15" ht="13.5" thickBot="1">
+      <c r="A31" s="60"/>
+      <c r="B31" s="61"/>
+      <c r="C31" s="61"/>
+      <c r="D31" s="61"/>
+      <c r="E31" s="61"/>
+      <c r="F31" s="61"/>
+      <c r="G31" s="61"/>
+      <c r="H31" s="61"/>
+      <c r="I31" s="61"/>
+      <c r="J31" s="61"/>
+      <c r="K31" s="61"/>
+      <c r="L31" s="61"/>
+      <c r="M31" s="61"/>
+      <c r="N31" s="61"/>
+      <c r="O31" s="62"/>
+    </row>
+    <row r="32" spans="1:15" ht="4.5" customHeight="1" thickBot="1">
+      <c r="B32" s="13"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="42"/>
+      <c r="E32" s="42"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="42"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="41"/>
+      <c r="J32" s="41"/>
+      <c r="K32" s="41"/>
+      <c r="L32" s="41"/>
+      <c r="M32" s="41"/>
+      <c r="N32" s="41"/>
+    </row>
+    <row r="33" spans="2:14">
+      <c r="B33" s="63"/>
+      <c r="C33" s="64"/>
+      <c r="D33" s="65"/>
+      <c r="H33" s="63"/>
+      <c r="I33" s="64"/>
+      <c r="J33" s="64"/>
+      <c r="K33" s="64"/>
+      <c r="L33" s="64"/>
+      <c r="M33" s="64"/>
+      <c r="N33" s="65"/>
+    </row>
+    <row r="34" spans="2:14">
+      <c r="B34" s="66"/>
+      <c r="C34" s="67"/>
+      <c r="D34" s="68"/>
+      <c r="H34" s="66"/>
+      <c r="I34" s="67"/>
+      <c r="J34" s="67"/>
+      <c r="K34" s="67"/>
+      <c r="L34" s="67"/>
+      <c r="M34" s="67"/>
+      <c r="N34" s="68"/>
+    </row>
+    <row r="35" spans="2:14">
+      <c r="B35" s="66"/>
+      <c r="C35" s="67"/>
+      <c r="D35" s="68"/>
+      <c r="H35" s="66"/>
+      <c r="I35" s="67"/>
+      <c r="J35" s="67"/>
+      <c r="K35" s="67"/>
+      <c r="L35" s="67"/>
+      <c r="M35" s="67"/>
+      <c r="N35" s="68"/>
+    </row>
+    <row r="36" spans="2:14" ht="13.5" thickBot="1">
+      <c r="B36" s="69"/>
+      <c r="C36" s="70"/>
+      <c r="D36" s="71"/>
+      <c r="H36" s="69"/>
+      <c r="I36" s="70"/>
+      <c r="J36" s="70"/>
+      <c r="K36" s="70"/>
+      <c r="L36" s="70"/>
+      <c r="M36" s="70"/>
+      <c r="N36" s="71"/>
+    </row>
+    <row r="37" spans="2:14">
+      <c r="B37" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" s="40"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="H22" s="128"/>
-      <c r="I22" s="95"/>
-      <c r="J22" s="96"/>
-      <c r="K22" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="L22" s="97"/>
-      <c r="M22" s="96"/>
-      <c r="N22" s="97"/>
-      <c r="O22" s="98"/>
-    </row>
-    <row r="23" spans="1:15">
-      <c r="A23" s="33"/>
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="127"/>
-      <c r="H23" s="128"/>
-      <c r="I23" s="91"/>
-      <c r="J23" s="92"/>
-      <c r="K23" s="8">
-        <v>23</v>
-      </c>
-      <c r="L23" s="93"/>
-      <c r="M23" s="92"/>
-      <c r="N23" s="93"/>
-      <c r="O23" s="94"/>
-    </row>
-    <row r="24" spans="1:15" ht="13.5" thickBot="1">
-      <c r="A24" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24" s="29"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="127"/>
-      <c r="H24" s="128"/>
-      <c r="I24" s="91"/>
-      <c r="J24" s="92"/>
-      <c r="K24" s="8">
-        <v>8</v>
-      </c>
-      <c r="L24" s="93"/>
-      <c r="M24" s="92"/>
-      <c r="N24" s="93"/>
-      <c r="O24" s="94"/>
-    </row>
-    <row r="25" spans="1:15">
-      <c r="A25" s="135"/>
-      <c r="B25" s="136"/>
-      <c r="C25" s="136"/>
-      <c r="D25" s="136"/>
-      <c r="E25" s="136"/>
-      <c r="F25" s="137"/>
-      <c r="G25" s="127"/>
-      <c r="H25" s="128"/>
-      <c r="I25" s="91"/>
-      <c r="J25" s="92"/>
-      <c r="K25" s="8">
-        <v>5</v>
-      </c>
-      <c r="L25" s="93"/>
-      <c r="M25" s="92"/>
-      <c r="N25" s="93"/>
-      <c r="O25" s="94"/>
-    </row>
-    <row r="26" spans="1:15" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A26" s="138"/>
-      <c r="B26" s="139"/>
-      <c r="C26" s="139"/>
-      <c r="D26" s="139"/>
-      <c r="E26" s="139"/>
-      <c r="F26" s="140"/>
-      <c r="G26" s="129"/>
-      <c r="H26" s="130"/>
-      <c r="I26" s="122"/>
-      <c r="J26" s="123"/>
-      <c r="K26" s="17">
-        <v>0</v>
-      </c>
-      <c r="L26" s="126"/>
-      <c r="M26" s="123"/>
-      <c r="N26" s="126"/>
-      <c r="O26" s="131"/>
-    </row>
-    <row r="27" spans="1:15" ht="4.5" customHeight="1" thickBot="1">
-      <c r="A27" s="34"/>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="11"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10"/>
-      <c r="N27" s="10"/>
-      <c r="O27" s="10"/>
-    </row>
-    <row r="28" spans="1:15">
-      <c r="A28" s="141" t="s">
-        <v>20</v>
-      </c>
-      <c r="B28" s="142"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="145"/>
-      <c r="E28" s="145"/>
-      <c r="F28" s="146"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18"/>
-      <c r="M28" s="18"/>
-      <c r="N28" s="18"/>
-      <c r="O28" s="18"/>
-    </row>
-    <row r="29" spans="1:15" ht="13.5" thickBot="1">
-      <c r="A29" s="143"/>
-      <c r="B29" s="144"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="147"/>
-      <c r="E29" s="147"/>
-      <c r="F29" s="148"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="18"/>
-      <c r="L29" s="18"/>
-      <c r="M29" s="18"/>
-      <c r="N29" s="18"/>
-      <c r="O29" s="18"/>
-    </row>
-    <row r="30" spans="1:15" ht="3.75" customHeight="1" thickBot="1">
-      <c r="A30" s="37"/>
-      <c r="B30" s="38"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="19"/>
-      <c r="K30" s="19"/>
-      <c r="L30" s="19"/>
-      <c r="M30" s="19"/>
-      <c r="N30" s="19"/>
-      <c r="O30" s="19"/>
-    </row>
-    <row r="31" spans="1:15">
-      <c r="A31" s="149" t="s">
-        <v>37</v>
-      </c>
-      <c r="B31" s="150"/>
-      <c r="C31" s="150"/>
-      <c r="D31" s="150"/>
-      <c r="E31" s="150"/>
-      <c r="F31" s="150"/>
-      <c r="G31" s="150"/>
-      <c r="H31" s="150"/>
-      <c r="I31" s="150"/>
-      <c r="J31" s="150"/>
-      <c r="K31" s="150"/>
-      <c r="L31" s="150"/>
-      <c r="M31" s="150"/>
-      <c r="N31" s="150"/>
-      <c r="O31" s="151"/>
-    </row>
-    <row r="32" spans="1:15" ht="13.5" thickBot="1">
-      <c r="A32" s="152"/>
-      <c r="B32" s="153"/>
-      <c r="C32" s="153"/>
-      <c r="D32" s="153"/>
-      <c r="E32" s="153"/>
-      <c r="F32" s="153"/>
-      <c r="G32" s="153"/>
-      <c r="H32" s="153"/>
-      <c r="I32" s="153"/>
-      <c r="J32" s="153"/>
-      <c r="K32" s="153"/>
-      <c r="L32" s="153"/>
-      <c r="M32" s="153"/>
-      <c r="N32" s="153"/>
-      <c r="O32" s="154"/>
-    </row>
-    <row r="33" spans="2:14" ht="4.5" customHeight="1" thickBot="1">
-      <c r="B33" s="14"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="134"/>
-      <c r="E33" s="134"/>
-      <c r="F33" s="134"/>
-      <c r="G33" s="134"/>
-      <c r="H33" s="134"/>
-      <c r="I33" s="133"/>
-      <c r="J33" s="133"/>
-      <c r="K33" s="133"/>
-      <c r="L33" s="133"/>
-      <c r="M33" s="133"/>
-      <c r="N33" s="133"/>
-    </row>
-    <row r="34" spans="2:14">
-      <c r="B34" s="155"/>
-      <c r="C34" s="156"/>
-      <c r="D34" s="157"/>
-      <c r="H34" s="155"/>
-      <c r="I34" s="156"/>
-      <c r="J34" s="156"/>
-      <c r="K34" s="156"/>
-      <c r="L34" s="156"/>
-      <c r="M34" s="156"/>
-      <c r="N34" s="157"/>
-    </row>
-    <row r="35" spans="2:14">
-      <c r="B35" s="158"/>
-      <c r="C35" s="159"/>
-      <c r="D35" s="160"/>
-      <c r="H35" s="158"/>
-      <c r="I35" s="159"/>
-      <c r="J35" s="159"/>
-      <c r="K35" s="159"/>
-      <c r="L35" s="159"/>
-      <c r="M35" s="159"/>
-      <c r="N35" s="160"/>
-    </row>
-    <row r="36" spans="2:14">
-      <c r="B36" s="158"/>
-      <c r="C36" s="159"/>
-      <c r="D36" s="160"/>
-      <c r="H36" s="158"/>
-      <c r="I36" s="159"/>
-      <c r="J36" s="159"/>
-      <c r="K36" s="159"/>
-      <c r="L36" s="159"/>
-      <c r="M36" s="159"/>
-      <c r="N36" s="160"/>
-    </row>
-    <row r="37" spans="2:14" ht="13.5" thickBot="1">
-      <c r="B37" s="161"/>
-      <c r="C37" s="162"/>
-      <c r="D37" s="163"/>
-      <c r="H37" s="161"/>
-      <c r="I37" s="162"/>
-      <c r="J37" s="162"/>
-      <c r="K37" s="162"/>
-      <c r="L37" s="162"/>
-      <c r="M37" s="162"/>
-      <c r="N37" s="163"/>
-    </row>
-    <row r="38" spans="2:14">
-      <c r="B38" s="132" t="s">
-        <v>14</v>
-      </c>
-      <c r="C38" s="132"/>
-      <c r="D38" s="132"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="132" t="s">
-        <v>15</v>
-      </c>
-      <c r="I38" s="132"/>
-      <c r="J38" s="132"/>
-      <c r="K38" s="132"/>
-      <c r="L38" s="132"/>
-      <c r="M38" s="132"/>
-      <c r="N38" s="132"/>
+      <c r="I37" s="40"/>
+      <c r="J37" s="40"/>
+      <c r="K37" s="40"/>
+      <c r="L37" s="40"/>
+      <c r="M37" s="40"/>
+      <c r="N37" s="40"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="82">
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="H38:N38"/>
-    <mergeCell ref="I33:N33"/>
-    <mergeCell ref="D33:H33"/>
-    <mergeCell ref="A25:F26"/>
-    <mergeCell ref="A28:B29"/>
-    <mergeCell ref="D28:F29"/>
-    <mergeCell ref="A31:O32"/>
-    <mergeCell ref="B34:D37"/>
-    <mergeCell ref="H34:N37"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="E13:E15"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="L26:M26"/>
+  <mergeCells count="80">
+    <mergeCell ref="E1:K1"/>
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="A1:D4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A7:E9"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F7:O9"/>
+    <mergeCell ref="F10:O10"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="F11:O11"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="E3:K3"/>
+    <mergeCell ref="E4:K4"/>
+    <mergeCell ref="L3:O3"/>
+    <mergeCell ref="L4:O4"/>
+    <mergeCell ref="E2:K2"/>
+    <mergeCell ref="I6:O6"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="F13:F15"/>
+    <mergeCell ref="N13:O14"/>
+    <mergeCell ref="I13:J14"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="G13:H14"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H25"/>
     <mergeCell ref="N25:O25"/>
-    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="N17:O17"/>
     <mergeCell ref="G16:H16"/>
@@ -2419,49 +2415,40 @@
     <mergeCell ref="N20:O20"/>
     <mergeCell ref="G19:H19"/>
     <mergeCell ref="N19:O19"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="B17:B18"/>
     <mergeCell ref="N23:O23"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H26"/>
-    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="H37:N37"/>
+    <mergeCell ref="I32:N32"/>
+    <mergeCell ref="D32:H32"/>
+    <mergeCell ref="A24:F25"/>
+    <mergeCell ref="A27:B28"/>
+    <mergeCell ref="D27:F28"/>
+    <mergeCell ref="A30:O31"/>
+    <mergeCell ref="B33:D36"/>
+    <mergeCell ref="H33:N36"/>
     <mergeCell ref="I24:J24"/>
     <mergeCell ref="L24:M24"/>
-    <mergeCell ref="L3:O3"/>
-    <mergeCell ref="L4:O4"/>
-    <mergeCell ref="E2:K2"/>
-    <mergeCell ref="I6:O6"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="F13:F15"/>
-    <mergeCell ref="N13:O14"/>
-    <mergeCell ref="I13:J14"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="G13:H14"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="E1:K1"/>
-    <mergeCell ref="L1:O1"/>
-    <mergeCell ref="A1:D4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A7:E9"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F7:O9"/>
-    <mergeCell ref="F10:O10"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="F11:O11"/>
-    <mergeCell ref="L2:O2"/>
-    <mergeCell ref="E3:K3"/>
-    <mergeCell ref="E4:K4"/>
+    <mergeCell ref="H27:O28"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.31496062992125984" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="79" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>

</xml_diff>